<commit_message>
feat(source): set some variables to not being tuned and add saturation
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables_20.xlsx
+++ b/JupyterNotebooks/variables_20.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C4961-9B68-431E-9C35-64D1CE64904A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8308B45-C777-490E-9A45-62066F4BC660}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Diatoms1: [Cyclotella nana]</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -670,7 +673,7 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -695,7 +698,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F7">
         <v>0.05</v>
@@ -1000,7 +1003,7 @@
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F19">
         <v>0.08</v>
@@ -1023,7 +1026,7 @@
         <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F20">
         <v>1.7999999999999999E-2</v>

</xml_diff>

<commit_message>
feat(source): remove saturation from tuned parameters
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables_20.xlsx
+++ b/JupyterNotebooks/variables_20.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8308B45-C777-490E-9A45-62066F4BC660}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F06F28A-CB97-4E3D-89BF-AEA228E27894}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -798,7 +798,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F11">
         <v>11</v>
@@ -1046,7 +1046,7 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F21">
         <v>22.5</v>

</xml_diff>

<commit_message>
fix(source): solve numeric formatting problem
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables_20.xlsx
+++ b/JupyterNotebooks/variables_20.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F06F28A-CB97-4E3D-89BF-AEA228E27894}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643D01BB-B8C4-4893-B9D9-68E123F1CBC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -99,21 +99,6 @@
     <t>Hard Max</t>
   </si>
   <si>
-    <t>0,2</t>
-  </si>
-  <si>
-    <t>0,04</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>0,001</t>
-  </si>
-  <si>
-    <t>1,52</t>
-  </si>
-  <si>
     <t>"TOpt"</t>
   </si>
   <si>
@@ -126,49 +111,22 @@
     <t>"P2Org"</t>
   </si>
   <si>
-    <t>0,005</t>
-  </si>
-  <si>
-    <t>0,01</t>
-  </si>
-  <si>
     <t>"KSed"</t>
   </si>
   <si>
-    <t>0,07</t>
-  </si>
-  <si>
-    <t>0,32</t>
-  </si>
-  <si>
     <t>"ESed"</t>
   </si>
   <si>
-    <t>0,05</t>
-  </si>
-  <si>
     <t>"ECoeffPhyto"</t>
   </si>
   <si>
     <t>"KResp"</t>
   </si>
   <si>
-    <t>0,34</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>1,55</t>
-  </si>
-  <si>
     <t>Cyclotella Nana</t>
   </si>
   <si>
     <t>Diatoms1: [Cyclotella nana]</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -184,12 +142,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,9 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -491,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -561,13 +528,13 @@
       <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
+      <c r="I2" s="1">
+        <v>0.2</v>
       </c>
       <c r="J2" s="1">
         <v>8</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -591,13 +558,13 @@
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1"/>
+      <c r="I3" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -621,11 +588,11 @@
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
+      <c r="I4" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.52</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -670,10 +637,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -695,10 +662,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>0.05</v>
@@ -718,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -743,7 +710,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -754,11 +721,11 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>34</v>
+      <c r="I9" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.01</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -770,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -779,11 +746,11 @@
         <v>3.1E-2</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>37</v>
+      <c r="I10" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.32</v>
       </c>
       <c r="K10" s="1"/>
     </row>
@@ -798,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>11</v>
@@ -822,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -833,11 +800,11 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>24</v>
+      <c r="I12" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.2</v>
       </c>
       <c r="K12" s="1"/>
     </row>
@@ -849,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -872,7 +839,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -889,10 +856,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -906,19 +873,19 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" t="s">
-        <v>43</v>
+      <c r="I15">
+        <v>0.34</v>
+      </c>
+      <c r="J15">
+        <v>3.4</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -932,20 +899,20 @@
       <c r="H16" s="1">
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>44</v>
+      <c r="I16" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.55</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -969,13 +936,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -994,16 +961,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <v>0.08</v>
@@ -1017,16 +984,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F20">
         <v>1.7999999999999999E-2</v>
@@ -1037,16 +1004,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F21">
         <v>22.5</v>

</xml_diff>